<commit_message>
+ jury excel update
</commit_message>
<xml_diff>
--- a/DeliveryProject_linux/excel/jury.xlsx
+++ b/DeliveryProject_linux/excel/jury.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carloscampos/Desktop/DeliveryProject_linux/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Campos\Desktop\Delivery\CMA.ISMAI.Delivery\DeliveryProject_windows\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097BE6F6-9639-C048-B893-2C28B7D2F740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9065CCF9-CA20-4E1A-9F93-339333FBF18F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5500" windowWidth="21600" windowHeight="11380" xr2:uid="{9FCB5A71-D7F2-499A-946F-5044815C75BC}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="16200" windowHeight="9360" xr2:uid="{9FCB5A71-D7F2-499A-946F-5044815C75BC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Diretores de departamento" sheetId="3" r:id="rId1"/>
+    <sheet name="juri" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -424,13 +424,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -447,7 +447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -464,10 +464,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
     </row>
   </sheetData>

</xml_diff>